<commit_message>
Se realizan últimos ajustes de entrega de reto
</commit_message>
<xml_diff>
--- a/RETO PRUEBAS MANUALES/Informe de avance RETO.xlsx
+++ b/RETO PRUEBAS MANUALES/Informe de avance RETO.xlsx
@@ -5,19 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\io\Desktop\RETO QA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\io\Desktop\RETO PRUEBAS MANUALES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EED99736-704F-4228-BA96-4484AD8CB545}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFEBF99A-4ECB-405D-B22A-6F4C0F323A5B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{51503347-54DB-4609-BF7A-D9CC5CBC859E}"/>
   </bookViews>
   <sheets>
     <sheet name="INFORME DE AVANCE" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>INFORME DE AVANCE RETO PRUEBAS MANUALES</t>
   </si>
@@ -343,6 +340,14 @@
       <t xml:space="preserve"> Francy Julieth Ramirez Rodriguez</t>
     </r>
   </si>
+  <si>
+    <t>Total de casos de prueba ejecutados: 15
+Exitosos: 14
+Fallidos: 1
+Bloqueados: 0
+Pendientes: 15
+Bugs reportados: 4</t>
+  </si>
 </sst>
 </file>
 
@@ -514,9 +519,72 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -545,9 +613,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -575,36 +640,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -631,89 +666,68 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3395,15 +3409,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>125144</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>51670</xdr:rowOff>
+      <xdr:colOff>210869</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>175495</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>552449</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>352425</xdr:rowOff>
+      <xdr:colOff>638174</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>476250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3433,7 +3447,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="887144" y="8948020"/>
+          <a:off x="972869" y="10548220"/>
           <a:ext cx="10466655" cy="6568205"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3454,19 +3468,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Gestion de incidentes"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3766,10 +3767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BA9DE49-204A-453B-B59D-E6F70F7FD026}">
-  <dimension ref="B1:O43"/>
+  <dimension ref="B1:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3785,602 +3786,647 @@
   <sheetData>
     <row r="1" spans="2:15" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="4"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="25"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="7"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="28"/>
     </row>
     <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="10"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="31"/>
     </row>
     <row r="5" spans="2:15" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="14"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="34"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="15"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="17"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="37"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="15"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="17"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="37"/>
     </row>
     <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="20"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="40"/>
     </row>
     <row r="10" spans="2:15" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="33"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="43"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="34"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="36"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="45"/>
+      <c r="M12" s="46"/>
     </row>
     <row r="13" spans="2:15" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="34"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="36"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="45"/>
+      <c r="K13" s="45"/>
+      <c r="L13" s="45"/>
+      <c r="M13" s="46"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="34"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="36"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="45"/>
+      <c r="K14" s="45"/>
+      <c r="L14" s="45"/>
+      <c r="M14" s="46"/>
       <c r="O14" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="2:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="34"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="36"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="45"/>
+      <c r="K15" s="45"/>
+      <c r="L15" s="45"/>
+      <c r="M15" s="46"/>
       <c r="O15" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="2:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="34"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="35"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="36"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="45"/>
+      <c r="K16" s="45"/>
+      <c r="L16" s="45"/>
+      <c r="M16" s="46"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="34"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="36"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="45"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="45"/>
+      <c r="M17" s="46"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="34"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="36"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="45"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="45"/>
+      <c r="M18" s="46"/>
     </row>
     <row r="19" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="34"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="35"/>
-      <c r="M19" s="36"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="45"/>
+      <c r="K19" s="45"/>
+      <c r="L19" s="45"/>
+      <c r="M19" s="46"/>
     </row>
     <row r="20" spans="2:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="34"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="35"/>
-      <c r="K20" s="35"/>
-      <c r="L20" s="35"/>
-      <c r="M20" s="36"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="45"/>
+      <c r="K20" s="45"/>
+      <c r="L20" s="45"/>
+      <c r="M20" s="46"/>
     </row>
     <row r="21" spans="2:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="34"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="35"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="35"/>
-      <c r="M21" s="36"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="45"/>
+      <c r="J21" s="45"/>
+      <c r="K21" s="45"/>
+      <c r="L21" s="45"/>
+      <c r="M21" s="46"/>
     </row>
     <row r="22" spans="2:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="37"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="38"/>
-      <c r="L22" s="38"/>
-      <c r="M22" s="39"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="48"/>
+      <c r="K22" s="48"/>
+      <c r="L22" s="48"/>
+      <c r="M22" s="49"/>
     </row>
     <row r="23" spans="2:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="21" t="s">
+      <c r="C23" s="60"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="41"/>
-      <c r="J23" s="21" t="s">
+      <c r="G23" s="52"/>
+      <c r="H23" s="52"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="K23" s="22"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="23"/>
+      <c r="K23" s="52"/>
+      <c r="L23" s="52"/>
+      <c r="M23" s="53"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="42"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="44"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="43"/>
-      <c r="I24" s="44"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="25"/>
-      <c r="M24" s="26"/>
+      <c r="B24" s="62"/>
+      <c r="C24" s="63"/>
+      <c r="D24" s="63"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="55"/>
+      <c r="H24" s="55"/>
+      <c r="I24" s="56"/>
+      <c r="J24" s="54"/>
+      <c r="K24" s="55"/>
+      <c r="L24" s="55"/>
+      <c r="M24" s="56"/>
     </row>
-    <row r="25" spans="2:13" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="42"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="44"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="25"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="26"/>
+    <row r="25" spans="2:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="62"/>
+      <c r="C25" s="63"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="55"/>
+      <c r="H25" s="55"/>
+      <c r="I25" s="56"/>
+      <c r="J25" s="54"/>
+      <c r="K25" s="55"/>
+      <c r="L25" s="55"/>
+      <c r="M25" s="56"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="42"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="43"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="44"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="25"/>
-      <c r="L26" s="25"/>
-      <c r="M26" s="26"/>
+      <c r="B26" s="62"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="55"/>
+      <c r="H26" s="55"/>
+      <c r="I26" s="56"/>
+      <c r="J26" s="54"/>
+      <c r="K26" s="55"/>
+      <c r="L26" s="55"/>
+      <c r="M26" s="56"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="42"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="24"/>
-      <c r="K27" s="25"/>
-      <c r="L27" s="25"/>
-      <c r="M27" s="26"/>
+    <row r="27" spans="2:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="62"/>
+      <c r="C27" s="63"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="64"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="55"/>
+      <c r="H27" s="55"/>
+      <c r="I27" s="56"/>
+      <c r="J27" s="54"/>
+      <c r="K27" s="55"/>
+      <c r="L27" s="55"/>
+      <c r="M27" s="56"/>
     </row>
-    <row r="28" spans="2:13" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="45"/>
-      <c r="C28" s="46"/>
-      <c r="D28" s="46"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="46"/>
-      <c r="H28" s="46"/>
-      <c r="I28" s="47"/>
-      <c r="J28" s="27"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="29"/>
+    <row r="28" spans="2:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="62"/>
+      <c r="C28" s="63"/>
+      <c r="D28" s="63"/>
+      <c r="E28" s="64"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="55"/>
+      <c r="H28" s="55"/>
+      <c r="I28" s="56"/>
+      <c r="J28" s="54"/>
+      <c r="K28" s="55"/>
+      <c r="L28" s="55"/>
+      <c r="M28" s="56"/>
     </row>
-    <row r="29" spans="2:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="48" t="s">
+    <row r="29" spans="2:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="62"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="64"/>
+      <c r="F29" s="54"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="56"/>
+      <c r="J29" s="54"/>
+      <c r="K29" s="55"/>
+      <c r="L29" s="55"/>
+      <c r="M29" s="56"/>
+    </row>
+    <row r="30" spans="2:13" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="65"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="58"/>
+      <c r="H30" s="58"/>
+      <c r="I30" s="59"/>
+      <c r="J30" s="57"/>
+      <c r="K30" s="58"/>
+      <c r="L30" s="58"/>
+      <c r="M30" s="59"/>
+    </row>
+    <row r="31" spans="2:13" ht="104.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="69"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="69"/>
+      <c r="F31" s="69"/>
+      <c r="G31" s="69"/>
+      <c r="H31" s="69"/>
+      <c r="I31" s="69"/>
+      <c r="J31" s="69"/>
+      <c r="K31" s="69"/>
+      <c r="L31" s="69"/>
+      <c r="M31" s="70"/>
+    </row>
+    <row r="32" spans="2:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="49"/>
-      <c r="D29" s="49"/>
-      <c r="E29" s="49"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="49"/>
-      <c r="H29" s="49"/>
-      <c r="I29" s="49"/>
-      <c r="J29" s="49"/>
-      <c r="K29" s="49"/>
-      <c r="L29" s="49"/>
-      <c r="M29" s="50"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="4"/>
     </row>
-    <row r="30" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="30" t="s">
+    <row r="33" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="51"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="51"/>
-      <c r="F30" s="51"/>
-      <c r="G30" s="51"/>
-      <c r="H30" s="51"/>
-      <c r="I30" s="51"/>
-      <c r="J30" s="51"/>
-      <c r="K30" s="51"/>
-      <c r="L30" s="51"/>
-      <c r="M30" s="52"/>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B31" s="53"/>
-      <c r="C31" s="54"/>
-      <c r="D31" s="54"/>
-      <c r="E31" s="54"/>
-      <c r="F31" s="54"/>
-      <c r="G31" s="54"/>
-      <c r="H31" s="54"/>
-      <c r="I31" s="54"/>
-      <c r="J31" s="54"/>
-      <c r="K31" s="54"/>
-      <c r="L31" s="54"/>
-      <c r="M31" s="55"/>
-    </row>
-    <row r="32" spans="2:13" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="53"/>
-      <c r="C32" s="54"/>
-      <c r="D32" s="54"/>
-      <c r="E32" s="54"/>
-      <c r="F32" s="54"/>
-      <c r="G32" s="54"/>
-      <c r="H32" s="54"/>
-      <c r="I32" s="54"/>
-      <c r="J32" s="54"/>
-      <c r="K32" s="54"/>
-      <c r="L32" s="54"/>
-      <c r="M32" s="55"/>
-    </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B33" s="53"/>
-      <c r="C33" s="54"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="54"/>
-      <c r="F33" s="54"/>
-      <c r="G33" s="54"/>
-      <c r="H33" s="54"/>
-      <c r="I33" s="54"/>
-      <c r="J33" s="54"/>
-      <c r="K33" s="54"/>
-      <c r="L33" s="54"/>
-      <c r="M33" s="55"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="7"/>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B34" s="53"/>
-      <c r="C34" s="54"/>
-      <c r="D34" s="54"/>
-      <c r="E34" s="54"/>
-      <c r="F34" s="54"/>
-      <c r="G34" s="54"/>
-      <c r="H34" s="54"/>
-      <c r="I34" s="54"/>
-      <c r="J34" s="54"/>
-      <c r="K34" s="54"/>
-      <c r="L34" s="54"/>
-      <c r="M34" s="55"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
+      <c r="M34" s="10"/>
     </row>
-    <row r="35" spans="2:13" ht="114" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="53"/>
-      <c r="C35" s="54"/>
-      <c r="D35" s="54"/>
-      <c r="E35" s="54"/>
-      <c r="F35" s="54"/>
-      <c r="G35" s="54"/>
-      <c r="H35" s="54"/>
-      <c r="I35" s="54"/>
-      <c r="J35" s="54"/>
-      <c r="K35" s="54"/>
-      <c r="L35" s="54"/>
-      <c r="M35" s="55"/>
+    <row r="35" spans="2:13" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="8"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="10"/>
     </row>
-    <row r="36" spans="2:13" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="53"/>
-      <c r="C36" s="54"/>
-      <c r="D36" s="54"/>
-      <c r="E36" s="54"/>
-      <c r="F36" s="54"/>
-      <c r="G36" s="54"/>
-      <c r="H36" s="54"/>
-      <c r="I36" s="54"/>
-      <c r="J36" s="54"/>
-      <c r="K36" s="54"/>
-      <c r="L36" s="54"/>
-      <c r="M36" s="55"/>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B36" s="8"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="10"/>
     </row>
-    <row r="37" spans="2:13" ht="152.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="53"/>
-      <c r="C37" s="54"/>
-      <c r="D37" s="54"/>
-      <c r="E37" s="54"/>
-      <c r="F37" s="54"/>
-      <c r="G37" s="54"/>
-      <c r="H37" s="54"/>
-      <c r="I37" s="54"/>
-      <c r="J37" s="54"/>
-      <c r="K37" s="54"/>
-      <c r="L37" s="54"/>
-      <c r="M37" s="55"/>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B37" s="8"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="10"/>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B38" s="53"/>
-      <c r="C38" s="54"/>
-      <c r="D38" s="54"/>
-      <c r="E38" s="54"/>
-      <c r="F38" s="54"/>
-      <c r="G38" s="54"/>
-      <c r="H38" s="54"/>
-      <c r="I38" s="54"/>
-      <c r="J38" s="54"/>
-      <c r="K38" s="54"/>
-      <c r="L38" s="54"/>
-      <c r="M38" s="55"/>
+    <row r="38" spans="2:13" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="8"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="10"/>
     </row>
-    <row r="39" spans="2:13" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="56"/>
-      <c r="C39" s="57"/>
-      <c r="D39" s="57"/>
-      <c r="E39" s="57"/>
-      <c r="F39" s="57"/>
-      <c r="G39" s="57"/>
-      <c r="H39" s="57"/>
-      <c r="I39" s="57"/>
-      <c r="J39" s="57"/>
-      <c r="K39" s="57"/>
-      <c r="L39" s="57"/>
-      <c r="M39" s="58"/>
+    <row r="39" spans="2:13" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="8"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="10"/>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B40" s="59" t="s">
+    <row r="40" spans="2:13" ht="152.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="8"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="10"/>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B41" s="8"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="9"/>
+      <c r="L41" s="9"/>
+      <c r="M41" s="10"/>
+    </row>
+    <row r="42" spans="2:13" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="11"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="12"/>
+      <c r="K42" s="12"/>
+      <c r="L42" s="12"/>
+      <c r="M42" s="13"/>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B43" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C40" s="60"/>
-      <c r="D40" s="60"/>
-      <c r="E40" s="60"/>
-      <c r="F40" s="60"/>
-      <c r="G40" s="60"/>
-      <c r="H40" s="60"/>
-      <c r="I40" s="60"/>
-      <c r="J40" s="60"/>
-      <c r="K40" s="60"/>
-      <c r="L40" s="60"/>
-      <c r="M40" s="61"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="15"/>
+      <c r="K43" s="15"/>
+      <c r="L43" s="15"/>
+      <c r="M43" s="16"/>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B41" s="62"/>
-      <c r="C41" s="63"/>
-      <c r="D41" s="63"/>
-      <c r="E41" s="63"/>
-      <c r="F41" s="63"/>
-      <c r="G41" s="63"/>
-      <c r="H41" s="63"/>
-      <c r="I41" s="63"/>
-      <c r="J41" s="63"/>
-      <c r="K41" s="63"/>
-      <c r="L41" s="63"/>
-      <c r="M41" s="64"/>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B44" s="17"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="18"/>
+      <c r="I44" s="18"/>
+      <c r="J44" s="18"/>
+      <c r="K44" s="18"/>
+      <c r="L44" s="18"/>
+      <c r="M44" s="19"/>
     </row>
-    <row r="42" spans="2:13" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="62"/>
-      <c r="C42" s="63"/>
-      <c r="D42" s="63"/>
-      <c r="E42" s="63"/>
-      <c r="F42" s="63"/>
-      <c r="G42" s="63"/>
-      <c r="H42" s="63"/>
-      <c r="I42" s="63"/>
-      <c r="J42" s="63"/>
-      <c r="K42" s="63"/>
-      <c r="L42" s="63"/>
-      <c r="M42" s="64"/>
+    <row r="45" spans="2:13" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="17"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
+      <c r="I45" s="18"/>
+      <c r="J45" s="18"/>
+      <c r="K45" s="18"/>
+      <c r="L45" s="18"/>
+      <c r="M45" s="19"/>
     </row>
-    <row r="43" spans="2:13" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="65"/>
-      <c r="C43" s="66"/>
-      <c r="D43" s="66"/>
-      <c r="E43" s="66"/>
-      <c r="F43" s="66"/>
-      <c r="G43" s="66"/>
-      <c r="H43" s="66"/>
-      <c r="I43" s="66"/>
-      <c r="J43" s="66"/>
-      <c r="K43" s="66"/>
-      <c r="L43" s="66"/>
-      <c r="M43" s="67"/>
+    <row r="46" spans="2:13" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="20"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
+      <c r="K46" s="21"/>
+      <c r="L46" s="21"/>
+      <c r="M46" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="B29:M29"/>
-    <mergeCell ref="B30:M39"/>
-    <mergeCell ref="B40:M43"/>
+  <mergeCells count="10">
+    <mergeCell ref="B32:M32"/>
+    <mergeCell ref="B33:M42"/>
+    <mergeCell ref="B43:M46"/>
     <mergeCell ref="B2:M4"/>
     <mergeCell ref="B6:M9"/>
     <mergeCell ref="B11:M22"/>
-    <mergeCell ref="B23:E28"/>
-    <mergeCell ref="F23:I28"/>
-    <mergeCell ref="J23:M28"/>
+    <mergeCell ref="B23:E30"/>
+    <mergeCell ref="F23:I30"/>
+    <mergeCell ref="J23:M30"/>
+    <mergeCell ref="B31:M31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>